<commit_message>
add script and data for Chinook figure 25 - total SEAK ER for CTC indicator stocks. with new 2025 data from PSC
</commit_message>
<xml_diff>
--- a/data-raw/cn_all_mort_new2025.xlsx
+++ b/data-raw/cn_all_mort_new2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/Alaskan-catch-of-BC-salmon/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1686583-FB12-9D4C-83E8-F15288C52DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E8F9AD-F375-EB46-974E-BDA928C06EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="500" windowWidth="26880" windowHeight="15940" xr2:uid="{9DF14ED9-0A62-154E-961C-EE083C2918EA}"/>
+    <workbookView xWindow="1920" yWindow="500" windowWidth="26880" windowHeight="15940" xr2:uid="{9DF14ED9-0A62-154E-961C-EE083C2918EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -402,9 +402,90 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="1" xr:uid="{26A891A1-BC41-D24B-A91E-5F8B6D1E9282}"/>
   </cellStyles>
-  <dxfs count="76">
+  <dxfs count="48">
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
@@ -609,256 +690,7 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -874,44 +706,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C110A3CB-75A0-2044-BB04-F273BF987E99}" name="Table1" displayName="Table1" ref="A1:AI901" totalsRowShown="0" dataDxfId="0" dataCellStyle="Normal 2 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C110A3CB-75A0-2044-BB04-F273BF987E99}" name="Table1" displayName="Table1" ref="A1:AI901" totalsRowShown="0" dataDxfId="47" dataCellStyle="Normal 2 2">
   <autoFilter ref="A1:AI901" xr:uid="{C110A3CB-75A0-2044-BB04-F273BF987E99}"/>
   <tableColumns count="35">
     <tableColumn id="1" xr3:uid="{B54EDF3E-0B5E-7C48-808B-D024C4D10377}" name="Stock"/>
     <tableColumn id="2" xr3:uid="{87E9BA4D-853D-904F-BC9E-BAF8CF8C30AE}" name="Region"/>
-    <tableColumn id="3" xr3:uid="{FB72A072-84E1-C24A-9C5F-8432A24F463C}" name="Catch.Year" dataDxfId="33" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="4" xr3:uid="{2CEFBC59-6FCD-204E-9827-D2D7D8BB99B1}" name="CWTs" dataDxfId="32" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="5" xr3:uid="{8110968C-A745-BB48-BBE2-006ACCCECEA8}" name="Ages" dataDxfId="31" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="6" xr3:uid="{1BB43558-0411-C648-97A2-8CC234F35900}" name="SEAK.Troll" dataDxfId="30" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="7" xr3:uid="{AD3EFE03-F4C4-2940-836E-3CD2B42FF072}" name="SEAK.Net" dataDxfId="29" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="8" xr3:uid="{45408834-20F9-9A47-B978-269C80117A85}" name="SEAK.Sport" dataDxfId="28" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="9" xr3:uid="{A7F7E0D5-6F24-2A4E-86C9-89367A827A62}" name="NBC.Troll" dataDxfId="27" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="10" xr3:uid="{B1A93BB6-F662-A14C-BB27-C5E180E4CB17}" name="NBC.Sport" dataDxfId="26" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="11" xr3:uid="{737F2988-8575-4140-A554-A8E0648C2585}" name="WCVI.Troll" dataDxfId="25" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="12" xr3:uid="{502A864E-A8DA-9540-9C2D-46BC91C8C01A}" name="WCVI.Sport" dataDxfId="24" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="13" xr3:uid="{3A72F8AC-3467-0143-9212-02BEFB31E61A}" name="ISBM.NCBC.Troll" dataDxfId="23" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="14" xr3:uid="{A1B34C72-13BB-5649-9201-6AE6A6A97A2A}" name="ISBM.NCBC.Net" dataDxfId="22" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="15" xr3:uid="{25B66711-5150-2C4A-B4F3-9090668C7416}" name="ISBM.NCBC.Sport" dataDxfId="21" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="16" xr3:uid="{0B3DCB28-CFAD-4848-8ED0-6CD34982C484}" name="ISBM.SBC.Troll" dataDxfId="20" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="17" xr3:uid="{F84CB47C-A06B-4B4B-A3FF-23DFC4B94A37}" name="ISBM.SBC.Net" dataDxfId="19" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="18" xr3:uid="{D628DD0B-FD79-2C43-8686-223ACA55CAF9}" name="ISBM.SBC.Sport" dataDxfId="18" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="19" xr3:uid="{A739E302-9055-8F4E-8ED9-FAFF0F9DE6C4}" name="ISBM.NF.Troll" dataDxfId="17" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="20" xr3:uid="{79530165-EA12-794D-8B39-0C91185C0B8B}" name="ISBM.NF.Sport" dataDxfId="16" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="21" xr3:uid="{838D0147-03C4-EA41-95EA-4C1AD09133EB}" name="ISBM.SF.Troll" dataDxfId="15" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="22" xr3:uid="{D82F43EC-64E5-4C4D-B04C-EC168BC503BC}" name="ISBM.SF.Sport" dataDxfId="14" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="23" xr3:uid="{189FC75C-6B08-5A46-9D7B-D43416ABCCD5}" name="ISBM.WAC.Net" dataDxfId="13" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="24" xr3:uid="{DA9454F8-90DC-5544-BD5D-4552C511158C}" name="ISBM.PS.Net" dataDxfId="12" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="25" xr3:uid="{015349A7-AC01-A640-A1FF-77793D541774}" name="ISBM.PS.Sport" dataDxfId="11" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="26" xr3:uid="{5508941F-DA13-8A4D-91AD-1C2F256FB82A}" name="Term.SEAK.Troll" dataDxfId="10" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="27" xr3:uid="{9EDA29B9-0F9F-EF44-98DF-723FA6EFFC16}" name="Term.SEAK.Net" dataDxfId="9" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="28" xr3:uid="{DBBF0A06-9658-834E-A531-2039F1252B7F}" name="Term.SEAK.Sport" dataDxfId="8" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="29" xr3:uid="{4A3E0557-8316-A345-A70E-3F7BDAFCD3E3}" name="Term.CAN.Net" dataDxfId="7" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="30" xr3:uid="{A4A3E7C0-3591-BE41-9BCA-9DAD3FD88CE8}" name="Term.CAN.Sport" dataDxfId="6" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="31" xr3:uid="{86E659A9-1611-D24D-BCAD-E36029E1E641}" name="Term.SUS.Troll" dataDxfId="5" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="32" xr3:uid="{35852B63-DA32-2540-A902-420AB3E588AD}" name="Term.SUS.Net" dataDxfId="4" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="33" xr3:uid="{253640FC-5290-214B-A938-E95880B6626B}" name="Term.SUS.Sport" dataDxfId="3" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="34" xr3:uid="{8108456E-7B6E-194A-BEB1-32B1738A73E0}" name="Stray" dataDxfId="2" dataCellStyle="Normal 2 2"/>
-    <tableColumn id="35" xr3:uid="{1933F1A5-B6F6-484F-9917-4CDC76691773}" name="Escapement" dataDxfId="1" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="3" xr3:uid="{FB72A072-84E1-C24A-9C5F-8432A24F463C}" name="Catch.Year" dataDxfId="46" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="4" xr3:uid="{2CEFBC59-6FCD-204E-9827-D2D7D8BB99B1}" name="CWTs" dataDxfId="45" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="5" xr3:uid="{8110968C-A745-BB48-BBE2-006ACCCECEA8}" name="Ages" dataDxfId="44" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="6" xr3:uid="{1BB43558-0411-C648-97A2-8CC234F35900}" name="SEAK.Troll" dataDxfId="43" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="7" xr3:uid="{AD3EFE03-F4C4-2940-836E-3CD2B42FF072}" name="SEAK.Net" dataDxfId="42" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="8" xr3:uid="{45408834-20F9-9A47-B978-269C80117A85}" name="SEAK.Sport" dataDxfId="41" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="9" xr3:uid="{A7F7E0D5-6F24-2A4E-86C9-89367A827A62}" name="NBC.Troll" dataDxfId="40" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="10" xr3:uid="{B1A93BB6-F662-A14C-BB27-C5E180E4CB17}" name="NBC.Sport" dataDxfId="39" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="11" xr3:uid="{737F2988-8575-4140-A554-A8E0648C2585}" name="WCVI.Troll" dataDxfId="38" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="12" xr3:uid="{502A864E-A8DA-9540-9C2D-46BC91C8C01A}" name="WCVI.Sport" dataDxfId="37" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="13" xr3:uid="{3A72F8AC-3467-0143-9212-02BEFB31E61A}" name="ISBM.NCBC.Troll" dataDxfId="36" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="14" xr3:uid="{A1B34C72-13BB-5649-9201-6AE6A6A97A2A}" name="ISBM.NCBC.Net" dataDxfId="35" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="15" xr3:uid="{25B66711-5150-2C4A-B4F3-9090668C7416}" name="ISBM.NCBC.Sport" dataDxfId="34" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="16" xr3:uid="{0B3DCB28-CFAD-4848-8ED0-6CD34982C484}" name="ISBM.SBC.Troll" dataDxfId="33" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="17" xr3:uid="{F84CB47C-A06B-4B4B-A3FF-23DFC4B94A37}" name="ISBM.SBC.Net" dataDxfId="32" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="18" xr3:uid="{D628DD0B-FD79-2C43-8686-223ACA55CAF9}" name="ISBM.SBC.Sport" dataDxfId="31" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="19" xr3:uid="{A739E302-9055-8F4E-8ED9-FAFF0F9DE6C4}" name="ISBM.NF.Troll" dataDxfId="30" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="20" xr3:uid="{79530165-EA12-794D-8B39-0C91185C0B8B}" name="ISBM.NF.Sport" dataDxfId="29" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="21" xr3:uid="{838D0147-03C4-EA41-95EA-4C1AD09133EB}" name="ISBM.SF.Troll" dataDxfId="28" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="22" xr3:uid="{D82F43EC-64E5-4C4D-B04C-EC168BC503BC}" name="ISBM.SF.Sport" dataDxfId="27" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="23" xr3:uid="{189FC75C-6B08-5A46-9D7B-D43416ABCCD5}" name="ISBM.WAC.Net" dataDxfId="26" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="24" xr3:uid="{DA9454F8-90DC-5544-BD5D-4552C511158C}" name="ISBM.PS.Net" dataDxfId="25" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="25" xr3:uid="{015349A7-AC01-A640-A1FF-77793D541774}" name="ISBM.PS.Sport" dataDxfId="24" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="26" xr3:uid="{5508941F-DA13-8A4D-91AD-1C2F256FB82A}" name="Term.SEAK.Troll" dataDxfId="23" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="27" xr3:uid="{9EDA29B9-0F9F-EF44-98DF-723FA6EFFC16}" name="Term.SEAK.Net" dataDxfId="22" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="28" xr3:uid="{DBBF0A06-9658-834E-A531-2039F1252B7F}" name="Term.SEAK.Sport" dataDxfId="21" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="29" xr3:uid="{4A3E0557-8316-A345-A70E-3F7BDAFCD3E3}" name="Term.CAN.Net" dataDxfId="20" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="30" xr3:uid="{A4A3E7C0-3591-BE41-9BCA-9DAD3FD88CE8}" name="Term.CAN.Sport" dataDxfId="19" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="31" xr3:uid="{86E659A9-1611-D24D-BCAD-E36029E1E641}" name="Term.SUS.Troll" dataDxfId="18" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="32" xr3:uid="{35852B63-DA32-2540-A902-420AB3E588AD}" name="Term.SUS.Net" dataDxfId="17" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="33" xr3:uid="{253640FC-5290-214B-A938-E95880B6626B}" name="Term.SUS.Sport" dataDxfId="16" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="34" xr3:uid="{8108456E-7B6E-194A-BEB1-32B1738A73E0}" name="Stray" dataDxfId="15" dataCellStyle="Normal 2 2"/>
+    <tableColumn id="35" xr3:uid="{1933F1A5-B6F6-484F-9917-4CDC76691773}" name="Escapement" dataDxfId="14" dataCellStyle="Normal 2 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1237,7 +1069,7 @@
   <dimension ref="A1:AI901"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -89760,172 +89592,60 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:AI496 M497:AI541 F542:AI631">
-    <cfRule type="expression" dxfId="75" priority="167">
-      <formula>$AH2="shade"</formula>
+  <conditionalFormatting sqref="F632:L766">
+    <cfRule type="expression" dxfId="13" priority="22">
+      <formula>$AH632="omit"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="168">
-      <formula>$AH2="omit"</formula>
+    <cfRule type="expression" dxfId="12" priority="21">
+      <formula>$AH632="shade"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F632:L676">
-    <cfRule type="expression" dxfId="73" priority="39">
-      <formula>$AH632="shade"</formula>
+  <conditionalFormatting sqref="F812:L901">
+    <cfRule type="expression" dxfId="11" priority="5">
+      <formula>$AH812="shade"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="40">
-      <formula>$AH632="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M632:Y676">
-    <cfRule type="expression" dxfId="71" priority="37">
-      <formula>$AH632="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="38">
-      <formula>$AH632="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z632:AI676">
-    <cfRule type="expression" dxfId="69" priority="35">
-      <formula>$AH632="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="68" priority="36">
-      <formula>$AH632="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F677:L721">
-    <cfRule type="expression" dxfId="67" priority="33">
-      <formula>$AH677="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="34">
-      <formula>$AH677="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M677:Y721">
-    <cfRule type="expression" dxfId="65" priority="31">
-      <formula>$AH677="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="32">
-      <formula>$AH677="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z677:AI721">
-    <cfRule type="expression" dxfId="63" priority="29">
-      <formula>$AH677="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="30">
-      <formula>$AH677="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F722:L765">
-    <cfRule type="expression" dxfId="61" priority="27">
-      <formula>$AH722="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="60" priority="28">
-      <formula>$AH722="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M722:Y765">
-    <cfRule type="expression" dxfId="59" priority="25">
-      <formula>$AH722="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="26">
-      <formula>$AH722="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z722:AI765">
-    <cfRule type="expression" dxfId="57" priority="23">
-      <formula>$AH722="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="24">
-      <formula>$AH722="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F766:L766">
-    <cfRule type="expression" dxfId="55" priority="21">
-      <formula>$AH766="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="22">
-      <formula>$AH766="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M766:Y766">
-    <cfRule type="expression" dxfId="53" priority="19">
-      <formula>$AH766="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="20">
-      <formula>$AH766="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z766:AI766">
-    <cfRule type="expression" dxfId="51" priority="17">
-      <formula>$AH766="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="50" priority="18">
-      <formula>$AH766="omit"</formula>
+    <cfRule type="expression" dxfId="10" priority="6">
+      <formula>$AH812="omit"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F767:Y811">
-    <cfRule type="expression" dxfId="49" priority="15">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>$AH767="shade"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="16">
+    <cfRule type="expression" dxfId="8" priority="16">
       <formula>$AH767="omit"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z767:AI811">
-    <cfRule type="expression" dxfId="47" priority="13">
-      <formula>$AH767="shade"</formula>
+  <conditionalFormatting sqref="F2:AI496 M497:AI541 F542:AI631">
+    <cfRule type="expression" dxfId="7" priority="168">
+      <formula>$AH2="omit"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="14">
-      <formula>$AH767="omit"</formula>
+    <cfRule type="expression" dxfId="6" priority="167">
+      <formula>$AH2="shade"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F812:L856">
-    <cfRule type="expression" dxfId="45" priority="11">
+  <conditionalFormatting sqref="M632:Y766">
+    <cfRule type="expression" dxfId="5" priority="20">
+      <formula>$AH632="omit"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="19">
+      <formula>$AH632="shade"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M812:Y901">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$AH812="omit"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$AH812="shade"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="12">
-      <formula>$AH812="omit"</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z632:AI901">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$AH632="shade"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M812:Y856">
-    <cfRule type="expression" dxfId="43" priority="9">
-      <formula>$AH812="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="10">
-      <formula>$AH812="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z812:AI856">
-    <cfRule type="expression" dxfId="41" priority="7">
-      <formula>$AH812="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="8">
-      <formula>$AH812="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F857:L901">
-    <cfRule type="expression" dxfId="39" priority="5">
-      <formula>$AH857="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="6">
-      <formula>$AH857="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M857:Y901">
-    <cfRule type="expression" dxfId="37" priority="3">
-      <formula>$AH857="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="4">
-      <formula>$AH857="omit"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z857:AI901">
-    <cfRule type="expression" dxfId="35" priority="1">
-      <formula>$AH857="shade"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="2">
-      <formula>$AH857="omit"</formula>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$AH632="omit"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>